<commit_message>
bom modified -> no V-Roll Kits -> bearings for v-rolls -> 4 wheels per carriage
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -57,9 +57,6 @@
     <t>Abstandsrollen PA M5 6mm, 10stk</t>
   </si>
   <si>
-    <t>V-Rollen Kit</t>
-  </si>
-  <si>
     <t>Pully 20Z GT2</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Summe:</t>
+  </si>
+  <si>
+    <t>Kugellager 625 2RS</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>4.5</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ref="E6:E16" si="0">C6*D6</f>
+        <f t="shared" ref="E6:E14" si="0">C6*D6</f>
         <v>9</v>
       </c>
     </row>
@@ -551,14 +551,14 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
         <v>1.49</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>5.96</v>
+        <v>11.92</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -584,17 +584,18 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>13</v>
+        <f>4*4*2</f>
+        <v>32</v>
       </c>
       <c r="D11" s="2">
-        <v>4.99</v>
+        <v>0.98</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>64.87</v>
+        <v>31.36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -602,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -620,7 +621,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>250</v>
@@ -638,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -653,11 +654,11 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1">
         <f>SUM(E5:E14)</f>
-        <v>197.13</v>
+        <v>169.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>